<commit_message>
creata pagina casi creati!!
</commit_message>
<xml_diff>
--- a/vodafone-selenium-form/excelVodafone.xlsx
+++ b/vodafone-selenium-form/excelVodafone.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t xml:space="preserve">informazioni</t>
   </si>
@@ -91,57 +91,64 @@
     <t xml:space="preserve">Dark Fiber</t>
   </si>
   <si>
+    <t xml:space="preserve">DARK FIBER DEGRADATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">333333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket di test,da non lavorare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">villa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pao.vi@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/lisa/vodafone_selenium/vodafone-selenium-form/src/main/resources/fileUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIRCUITO DOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:00-12:00 13:00-16:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDH/WDM - Punto Punto</t>
+  </si>
+  <si>
     <t xml:space="preserve">FWB_VOM _0000006083</t>
   </si>
   <si>
     <t xml:space="preserve">LA00239599 - VIA TRAVERSAGNA SUD SNC, 56019 VECCHIANO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DARK FIBER DEGRADATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket di test,da non lavorare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">villa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pao.vi@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/lisa/vodafone_selenium/vodafone-selenium-form/src/main/resources/fileUpload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DWDM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIRCUITO DOWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08:00-12:00 13:00-16:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDH/WDM - Punto Punto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -221,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +238,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,26 +266,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="30.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="9" style="1" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="1" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="49.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="23.48"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -305,7 +312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -327,7 +334,7 @@
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -342,7 +349,7 @@
       <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -361,30 +368,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>1234</v>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>28</v>
@@ -395,11 +396,11 @@
       <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="1" t="n">
-        <v>3333333333</v>
+      <c r="M3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>29</v>
@@ -407,26 +408,20 @@
       <c r="O3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="1" t="n">
-        <v>3333333333</v>
+      <c r="Q3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
@@ -436,11 +431,11 @@
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>1235</v>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
@@ -451,37 +446,27 @@
       <c r="K4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="1" t="n">
-        <v>3333333334</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="1" t="n">
-        <v>3333333334</v>
-      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>34</v>
@@ -490,13 +475,13 @@
         <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>1236</v>
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>28</v>
@@ -507,11 +492,11 @@
       <c r="K5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="1" t="n">
-        <v>3333333335</v>
+      <c r="M5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
@@ -519,16 +504,24 @@
       <c r="O5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="1" t="n">
-        <v>3333333335</v>
+      <c r="Q5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
@@ -539,9 +532,8 @@
     <hyperlink ref="L3" r:id="rId1" display="pao.vi@gmail.com"/>
     <hyperlink ref="P3" r:id="rId2" display="pao.vi@gmail.com"/>
     <hyperlink ref="L4" r:id="rId3" display="pao.vi@gmail.com"/>
-    <hyperlink ref="P4" r:id="rId4" display="pao.vi@gmail.com"/>
-    <hyperlink ref="L5" r:id="rId5" display="pao.vi@gmail.com"/>
-    <hyperlink ref="P5" r:id="rId6" display="pao.vi@gmail.com"/>
+    <hyperlink ref="L5" r:id="rId4" display="pao.vi@gmail.com"/>
+    <hyperlink ref="P5" r:id="rId5" display="pao.vi@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>